<commit_message>
removes trailing empty rows
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O253"/>
+  <dimension ref="A1:O232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14527,363 +14527,6 @@
       <c r="N232" t="inlineStr"/>
       <c r="O232" t="inlineStr"/>
     </row>
-    <row r="233">
-      <c r="A233" t="inlineStr"/>
-      <c r="B233" t="inlineStr"/>
-      <c r="C233" t="inlineStr"/>
-      <c r="D233" t="inlineStr"/>
-      <c r="E233" t="inlineStr"/>
-      <c r="F233" t="inlineStr"/>
-      <c r="G233" t="inlineStr"/>
-      <c r="H233" t="inlineStr"/>
-      <c r="I233" t="inlineStr"/>
-      <c r="J233" t="inlineStr"/>
-      <c r="K233" t="inlineStr"/>
-      <c r="L233" t="inlineStr"/>
-      <c r="M233" t="inlineStr"/>
-      <c r="N233" t="inlineStr"/>
-      <c r="O233" t="inlineStr"/>
-    </row>
-    <row r="234">
-      <c r="A234" t="inlineStr"/>
-      <c r="B234" t="inlineStr"/>
-      <c r="C234" t="inlineStr"/>
-      <c r="D234" t="inlineStr"/>
-      <c r="E234" t="inlineStr"/>
-      <c r="F234" t="inlineStr"/>
-      <c r="G234" t="inlineStr"/>
-      <c r="H234" t="inlineStr"/>
-      <c r="I234" t="inlineStr"/>
-      <c r="J234" t="inlineStr"/>
-      <c r="K234" t="inlineStr"/>
-      <c r="L234" t="inlineStr"/>
-      <c r="M234" t="inlineStr"/>
-      <c r="N234" t="inlineStr"/>
-      <c r="O234" t="inlineStr"/>
-    </row>
-    <row r="235">
-      <c r="A235" t="inlineStr"/>
-      <c r="B235" t="inlineStr"/>
-      <c r="C235" t="inlineStr"/>
-      <c r="D235" t="inlineStr"/>
-      <c r="E235" t="inlineStr"/>
-      <c r="F235" t="inlineStr"/>
-      <c r="G235" t="inlineStr"/>
-      <c r="H235" t="inlineStr"/>
-      <c r="I235" t="inlineStr"/>
-      <c r="J235" t="inlineStr"/>
-      <c r="K235" t="inlineStr"/>
-      <c r="L235" t="inlineStr"/>
-      <c r="M235" t="inlineStr"/>
-      <c r="N235" t="inlineStr"/>
-      <c r="O235" t="inlineStr"/>
-    </row>
-    <row r="236">
-      <c r="A236" t="inlineStr"/>
-      <c r="B236" t="inlineStr"/>
-      <c r="C236" t="inlineStr"/>
-      <c r="D236" t="inlineStr"/>
-      <c r="E236" t="inlineStr"/>
-      <c r="F236" t="inlineStr"/>
-      <c r="G236" t="inlineStr"/>
-      <c r="H236" t="inlineStr"/>
-      <c r="I236" t="inlineStr"/>
-      <c r="J236" t="inlineStr"/>
-      <c r="K236" t="inlineStr"/>
-      <c r="L236" t="inlineStr"/>
-      <c r="M236" t="inlineStr"/>
-      <c r="N236" t="inlineStr"/>
-      <c r="O236" t="inlineStr"/>
-    </row>
-    <row r="237">
-      <c r="A237" t="inlineStr"/>
-      <c r="B237" t="inlineStr"/>
-      <c r="C237" t="inlineStr"/>
-      <c r="D237" t="inlineStr"/>
-      <c r="E237" t="inlineStr"/>
-      <c r="F237" t="inlineStr"/>
-      <c r="G237" t="inlineStr"/>
-      <c r="H237" t="inlineStr"/>
-      <c r="I237" t="inlineStr"/>
-      <c r="J237" t="inlineStr"/>
-      <c r="K237" t="inlineStr"/>
-      <c r="L237" t="inlineStr"/>
-      <c r="M237" t="inlineStr"/>
-      <c r="N237" t="inlineStr"/>
-      <c r="O237" t="inlineStr"/>
-    </row>
-    <row r="238">
-      <c r="A238" t="inlineStr"/>
-      <c r="B238" t="inlineStr"/>
-      <c r="C238" t="inlineStr"/>
-      <c r="D238" t="inlineStr"/>
-      <c r="E238" t="inlineStr"/>
-      <c r="F238" t="inlineStr"/>
-      <c r="G238" t="inlineStr"/>
-      <c r="H238" t="inlineStr"/>
-      <c r="I238" t="inlineStr"/>
-      <c r="J238" t="inlineStr"/>
-      <c r="K238" t="inlineStr"/>
-      <c r="L238" t="inlineStr"/>
-      <c r="M238" t="inlineStr"/>
-      <c r="N238" t="inlineStr"/>
-      <c r="O238" t="inlineStr"/>
-    </row>
-    <row r="239">
-      <c r="A239" t="inlineStr"/>
-      <c r="B239" t="inlineStr"/>
-      <c r="C239" t="inlineStr"/>
-      <c r="D239" t="inlineStr"/>
-      <c r="E239" t="inlineStr"/>
-      <c r="F239" t="inlineStr"/>
-      <c r="G239" t="inlineStr"/>
-      <c r="H239" t="inlineStr"/>
-      <c r="I239" t="inlineStr"/>
-      <c r="J239" t="inlineStr"/>
-      <c r="K239" t="inlineStr"/>
-      <c r="L239" t="inlineStr"/>
-      <c r="M239" t="inlineStr"/>
-      <c r="N239" t="inlineStr"/>
-      <c r="O239" t="inlineStr"/>
-    </row>
-    <row r="240">
-      <c r="A240" t="inlineStr"/>
-      <c r="B240" t="inlineStr"/>
-      <c r="C240" t="inlineStr"/>
-      <c r="D240" t="inlineStr"/>
-      <c r="E240" t="inlineStr"/>
-      <c r="F240" t="inlineStr"/>
-      <c r="G240" t="inlineStr"/>
-      <c r="H240" t="inlineStr"/>
-      <c r="I240" t="inlineStr"/>
-      <c r="J240" t="inlineStr"/>
-      <c r="K240" t="inlineStr"/>
-      <c r="L240" t="inlineStr"/>
-      <c r="M240" t="inlineStr"/>
-      <c r="N240" t="inlineStr"/>
-      <c r="O240" t="inlineStr"/>
-    </row>
-    <row r="241">
-      <c r="A241" t="inlineStr"/>
-      <c r="B241" t="inlineStr"/>
-      <c r="C241" t="inlineStr"/>
-      <c r="D241" t="inlineStr"/>
-      <c r="E241" t="inlineStr"/>
-      <c r="F241" t="inlineStr"/>
-      <c r="G241" t="inlineStr"/>
-      <c r="H241" t="inlineStr"/>
-      <c r="I241" t="inlineStr"/>
-      <c r="J241" t="inlineStr"/>
-      <c r="K241" t="inlineStr"/>
-      <c r="L241" t="inlineStr"/>
-      <c r="M241" t="inlineStr"/>
-      <c r="N241" t="inlineStr"/>
-      <c r="O241" t="inlineStr"/>
-    </row>
-    <row r="242">
-      <c r="A242" t="inlineStr"/>
-      <c r="B242" t="inlineStr"/>
-      <c r="C242" t="inlineStr"/>
-      <c r="D242" t="inlineStr"/>
-      <c r="E242" t="inlineStr"/>
-      <c r="F242" t="inlineStr"/>
-      <c r="G242" t="inlineStr"/>
-      <c r="H242" t="inlineStr"/>
-      <c r="I242" t="inlineStr"/>
-      <c r="J242" t="inlineStr"/>
-      <c r="K242" t="inlineStr"/>
-      <c r="L242" t="inlineStr"/>
-      <c r="M242" t="inlineStr"/>
-      <c r="N242" t="inlineStr"/>
-      <c r="O242" t="inlineStr"/>
-    </row>
-    <row r="243">
-      <c r="A243" t="inlineStr"/>
-      <c r="B243" t="inlineStr"/>
-      <c r="C243" t="inlineStr"/>
-      <c r="D243" t="inlineStr"/>
-      <c r="E243" t="inlineStr"/>
-      <c r="F243" t="inlineStr"/>
-      <c r="G243" t="inlineStr"/>
-      <c r="H243" t="inlineStr"/>
-      <c r="I243" t="inlineStr"/>
-      <c r="J243" t="inlineStr"/>
-      <c r="K243" t="inlineStr"/>
-      <c r="L243" t="inlineStr"/>
-      <c r="M243" t="inlineStr"/>
-      <c r="N243" t="inlineStr"/>
-      <c r="O243" t="inlineStr"/>
-    </row>
-    <row r="244">
-      <c r="A244" t="inlineStr"/>
-      <c r="B244" t="inlineStr"/>
-      <c r="C244" t="inlineStr"/>
-      <c r="D244" t="inlineStr"/>
-      <c r="E244" t="inlineStr"/>
-      <c r="F244" t="inlineStr"/>
-      <c r="G244" t="inlineStr"/>
-      <c r="H244" t="inlineStr"/>
-      <c r="I244" t="inlineStr"/>
-      <c r="J244" t="inlineStr"/>
-      <c r="K244" t="inlineStr"/>
-      <c r="L244" t="inlineStr"/>
-      <c r="M244" t="inlineStr"/>
-      <c r="N244" t="inlineStr"/>
-      <c r="O244" t="inlineStr"/>
-    </row>
-    <row r="245">
-      <c r="A245" t="inlineStr"/>
-      <c r="B245" t="inlineStr"/>
-      <c r="C245" t="inlineStr"/>
-      <c r="D245" t="inlineStr"/>
-      <c r="E245" t="inlineStr"/>
-      <c r="F245" t="inlineStr"/>
-      <c r="G245" t="inlineStr"/>
-      <c r="H245" t="inlineStr"/>
-      <c r="I245" t="inlineStr"/>
-      <c r="J245" t="inlineStr"/>
-      <c r="K245" t="inlineStr"/>
-      <c r="L245" t="inlineStr"/>
-      <c r="M245" t="inlineStr"/>
-      <c r="N245" t="inlineStr"/>
-      <c r="O245" t="inlineStr"/>
-    </row>
-    <row r="246">
-      <c r="A246" t="inlineStr"/>
-      <c r="B246" t="inlineStr"/>
-      <c r="C246" t="inlineStr"/>
-      <c r="D246" t="inlineStr"/>
-      <c r="E246" t="inlineStr"/>
-      <c r="F246" t="inlineStr"/>
-      <c r="G246" t="inlineStr"/>
-      <c r="H246" t="inlineStr"/>
-      <c r="I246" t="inlineStr"/>
-      <c r="J246" t="inlineStr"/>
-      <c r="K246" t="inlineStr"/>
-      <c r="L246" t="inlineStr"/>
-      <c r="M246" t="inlineStr"/>
-      <c r="N246" t="inlineStr"/>
-      <c r="O246" t="inlineStr"/>
-    </row>
-    <row r="247">
-      <c r="A247" t="inlineStr"/>
-      <c r="B247" t="inlineStr"/>
-      <c r="C247" t="inlineStr"/>
-      <c r="D247" t="inlineStr"/>
-      <c r="E247" t="inlineStr"/>
-      <c r="F247" t="inlineStr"/>
-      <c r="G247" t="inlineStr"/>
-      <c r="H247" t="inlineStr"/>
-      <c r="I247" t="inlineStr"/>
-      <c r="J247" t="inlineStr"/>
-      <c r="K247" t="inlineStr"/>
-      <c r="L247" t="inlineStr"/>
-      <c r="M247" t="inlineStr"/>
-      <c r="N247" t="inlineStr"/>
-      <c r="O247" t="inlineStr"/>
-    </row>
-    <row r="248">
-      <c r="A248" t="inlineStr"/>
-      <c r="B248" t="inlineStr"/>
-      <c r="C248" t="inlineStr"/>
-      <c r="D248" t="inlineStr"/>
-      <c r="E248" t="inlineStr"/>
-      <c r="F248" t="inlineStr"/>
-      <c r="G248" t="inlineStr"/>
-      <c r="H248" t="inlineStr"/>
-      <c r="I248" t="inlineStr"/>
-      <c r="J248" t="inlineStr"/>
-      <c r="K248" t="inlineStr"/>
-      <c r="L248" t="inlineStr"/>
-      <c r="M248" t="inlineStr"/>
-      <c r="N248" t="inlineStr"/>
-      <c r="O248" t="inlineStr"/>
-    </row>
-    <row r="249">
-      <c r="A249" t="inlineStr"/>
-      <c r="B249" t="inlineStr"/>
-      <c r="C249" t="inlineStr"/>
-      <c r="D249" t="inlineStr"/>
-      <c r="E249" t="inlineStr"/>
-      <c r="F249" t="inlineStr"/>
-      <c r="G249" t="inlineStr"/>
-      <c r="H249" t="inlineStr"/>
-      <c r="I249" t="inlineStr"/>
-      <c r="J249" t="inlineStr"/>
-      <c r="K249" t="inlineStr"/>
-      <c r="L249" t="inlineStr"/>
-      <c r="M249" t="inlineStr"/>
-      <c r="N249" t="inlineStr"/>
-      <c r="O249" t="inlineStr"/>
-    </row>
-    <row r="250">
-      <c r="A250" t="inlineStr"/>
-      <c r="B250" t="inlineStr"/>
-      <c r="C250" t="inlineStr"/>
-      <c r="D250" t="inlineStr"/>
-      <c r="E250" t="inlineStr"/>
-      <c r="F250" t="inlineStr"/>
-      <c r="G250" t="inlineStr"/>
-      <c r="H250" t="inlineStr"/>
-      <c r="I250" t="inlineStr"/>
-      <c r="J250" t="inlineStr"/>
-      <c r="K250" t="inlineStr"/>
-      <c r="L250" t="inlineStr"/>
-      <c r="M250" t="inlineStr"/>
-      <c r="N250" t="inlineStr"/>
-      <c r="O250" t="inlineStr"/>
-    </row>
-    <row r="251">
-      <c r="A251" t="inlineStr"/>
-      <c r="B251" t="inlineStr"/>
-      <c r="C251" t="inlineStr"/>
-      <c r="D251" t="inlineStr"/>
-      <c r="E251" t="inlineStr"/>
-      <c r="F251" t="inlineStr"/>
-      <c r="G251" t="inlineStr"/>
-      <c r="H251" t="inlineStr"/>
-      <c r="I251" t="inlineStr"/>
-      <c r="J251" t="inlineStr"/>
-      <c r="K251" t="inlineStr"/>
-      <c r="L251" t="inlineStr"/>
-      <c r="M251" t="inlineStr"/>
-      <c r="N251" t="inlineStr"/>
-      <c r="O251" t="inlineStr"/>
-    </row>
-    <row r="252">
-      <c r="A252" t="inlineStr"/>
-      <c r="B252" t="inlineStr"/>
-      <c r="C252" t="inlineStr"/>
-      <c r="D252" t="inlineStr"/>
-      <c r="E252" t="inlineStr"/>
-      <c r="F252" t="inlineStr"/>
-      <c r="G252" t="inlineStr"/>
-      <c r="H252" t="inlineStr"/>
-      <c r="I252" t="inlineStr"/>
-      <c r="J252" t="inlineStr"/>
-      <c r="K252" t="inlineStr"/>
-      <c r="L252" t="inlineStr"/>
-      <c r="M252" t="inlineStr"/>
-      <c r="N252" t="inlineStr"/>
-      <c r="O252" t="inlineStr"/>
-    </row>
-    <row r="253">
-      <c r="A253" t="inlineStr"/>
-      <c r="B253" t="inlineStr"/>
-      <c r="C253" t="inlineStr"/>
-      <c r="D253" t="inlineStr"/>
-      <c r="E253" t="inlineStr"/>
-      <c r="F253" t="inlineStr"/>
-      <c r="G253" t="inlineStr"/>
-      <c r="H253" t="inlineStr"/>
-      <c r="I253" t="inlineStr"/>
-      <c r="J253" t="inlineStr"/>
-      <c r="K253" t="inlineStr"/>
-      <c r="L253" t="inlineStr"/>
-      <c r="M253" t="inlineStr"/>
-      <c r="N253" t="inlineStr"/>
-      <c r="O253" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>